<commit_message>
[pcb] Swap voltage divider resistors
</commit_message>
<xml_diff>
--- a/pcb/bom.xlsx
+++ b/pcb/bom.xlsx
@@ -445,43 +445,43 @@
     <t xml:space="preserve">https://www.mouser.pl/ProductDetail/71-CRCW0805-1.0M-E3</t>
   </si>
   <si>
+    <t xml:space="preserve">R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2kΩ, 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRCW080510K2FKEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.pl/ProductDetail/71-CRCW0805-10.2K-E3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18kΩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRCW080518K0FKEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.pl/ProductDetail/71-CRCW080518K0FKEA</t>
+  </si>
+  <si>
     <t xml:space="preserve">R2</t>
   </si>
   <si>
-    <t xml:space="preserve">10.2kΩ, 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRCW080510K2FKEA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.mouser.pl/ProductDetail/71-CRCW0805-10.2K-E3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18kΩ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRCW080518K0FKEA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.mouser.pl/ProductDetail/71-CRCW080518K0FKEA</t>
+    <t xml:space="preserve">53.6kΩ, 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRCW080553K6FKEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.pl/ProductDetail/71-CRCW080553K6FKEA</t>
   </si>
   <si>
     <t xml:space="preserve">R4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53.6kΩ, 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRCW080553K6FKEA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.mouser.pl/ProductDetail/71-CRCW080553K6FKEA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5</t>
   </si>
   <si>
     <t xml:space="preserve">20mΩ, 0.5W, 1%</t>
@@ -847,7 +847,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -880,10 +880,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -907,8 +903,8 @@
   </sheetPr>
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1841,7 +1837,7 @@
       <c r="G35" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="6" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2150,7 +2146,7 @@
       <c r="F47" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="G47" s="8" t="s">
         <v>212</v>
       </c>
       <c r="H47" s="6" t="s">

</xml_diff>

<commit_message>
[pcb] Change Schottky diode
</commit_message>
<xml_diff>
--- a/pcb/bom.xlsx
+++ b/pcb/bom.xlsx
@@ -236,16 +236,16 @@
     <t xml:space="preserve">D1</t>
   </si>
   <si>
-    <t xml:space="preserve">SKL34</t>
-  </si>
-  <si>
     <t xml:space="preserve">Diotec</t>
   </si>
   <si>
-    <t xml:space="preserve">SOD-123FL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.mouser.pl/ProductDetail/637-SKL34</t>
+    <t xml:space="preserve">SL52-3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.pl/ProductDetail/637-SL52-3G</t>
   </si>
   <si>
     <t xml:space="preserve">D2</t>
@@ -903,8 +903,8 @@
   </sheetPr>
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1202,13 +1202,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>56</v>
@@ -1231,7 +1231,7 @@
         <v>59</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>60</v>
@@ -2242,7 +2242,7 @@
     <hyperlink ref="H8" r:id="rId7" display="https://www.mouser.pl/ProductDetail/80-C0805C334K3R"/>
     <hyperlink ref="H9" r:id="rId8" display="https://www.mouser.pl/ProductDetail/80-C0805C300K3HACTU"/>
     <hyperlink ref="H10" r:id="rId9" display="https://www.mouser.pl/ProductDetail/80-T521T106M025ATE60"/>
-    <hyperlink ref="H11" r:id="rId10" display="https://www.mouser.pl/ProductDetail/637-SKL34"/>
+    <hyperlink ref="H11" r:id="rId10" display="https://www.mouser.pl/ProductDetail/637-SL52-3G"/>
     <hyperlink ref="H12" r:id="rId11" display="https://www.mouser.pl/ProductDetail/637-S1A"/>
     <hyperlink ref="H13" r:id="rId12" display="https://www.mouser.pl/ProductDetail/604-APT2012LZGCK"/>
     <hyperlink ref="H14" r:id="rId13" display="https://www.mouser.pl/ProductDetail/604-APT2012LSECKJ4RV"/>

</xml_diff>

<commit_message>
[pcb] Inductor upgrade, boost converter clean-up
</commit_message>
<xml_diff>
--- a/pcb/bom.xlsx
+++ b/pcb/bom.xlsx
@@ -397,13 +397,13 @@
     <t xml:space="preserve">Coilcraft</t>
   </si>
   <si>
-    <t xml:space="preserve">MSS1048-332NLC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10mm x 10,2mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.mouser.pl/ProductDetail/994-MSS1048-332NLC</t>
+    <t xml:space="preserve">MSS1260-332NLB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4747</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.pl/ProductDetail/994-MSS1260-332NLB</t>
   </si>
   <si>
     <t xml:space="preserve">M1, M2</t>
@@ -904,7 +904,7 @@
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2251,7 +2251,7 @@
     <hyperlink ref="H17" r:id="rId16" display="https://www.mouser.pl/ProductDetail/81-BLM21B221S"/>
     <hyperlink ref="H18" r:id="rId17" display="https://www.mouser.pl/ProductDetail/538-87834-0619"/>
     <hyperlink ref="H19" r:id="rId18" display="https://www.mouser.pl/ProductDetail/538-10-97-7086"/>
-    <hyperlink ref="H20" r:id="rId19" display="https://www.mouser.pl/ProductDetail/994-MSS1048-332NLC"/>
+    <hyperlink ref="H20" r:id="rId19" display="https://www.mouser.pl/ProductDetail/994-MSS1260-332NLB"/>
     <hyperlink ref="H21" r:id="rId20" display="https://www.tme.eu/pl/details/pololu-2364/silniki-dc/pololu/30-1-micro-metal-gearmotor-mp/"/>
     <hyperlink ref="H22" r:id="rId21" display="https://www.mouser.pl/ProductDetail/781-SI4368DY-T1-E3"/>
     <hyperlink ref="H23" r:id="rId22" display="https://www.mouser.pl/ProductDetail/71-CRCW0805-1.0M-E3"/>

</xml_diff>